<commit_message>
Carga de Documentos Entrega Segundo Corte -1
Se carga toda la documentacion en PDF, diagramas de secuencia y de
clases actializados
</commit_message>
<xml_diff>
--- a/Documentación/Justificación de Uso de Patrones/IGPA Justificación Final C2.xlsx
+++ b/Documentación/Justificación de Uso de Patrones/IGPA Justificación Final C2.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yerard\Documents\GitHub\ProyectoIGPA\Documentación\Justificación de Uso de Patrones\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="577"/>
   </bookViews>
   <sheets>
     <sheet name="Patrones de Diseño" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Patrones de Diseño'!$1:$7</definedName>
+  </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
@@ -148,8 +156,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -400,18 +408,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,16 +452,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -474,6 +482,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -565,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,9 +613,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -631,6 +648,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -806,345 +824,358 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21"/>
     <col min="2" max="3" width="11.5703125"/>
-    <col min="4" max="5" width="11.42578125" style="5"/>
-    <col min="6" max="6" width="69.140625" style="5"/>
+    <col min="4" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="69.140625" style="1"/>
     <col min="7" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" s="13" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="64.5" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="64.5" customHeight="1">
-      <c r="A10" s="14" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="76.5" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="66.75" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="66.75" customHeight="1">
-      <c r="A13" s="14" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="66.75" customHeight="1">
-      <c r="A14" s="14" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="53.25" customHeight="1">
-      <c r="A15" s="14" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="76.5" customHeight="1">
-      <c r="A16" s="14" t="s">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="55.5" customHeight="1">
-      <c r="A17" s="14" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="76.5" customHeight="1">
-      <c r="A18" s="14" t="s">
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="110.25" customHeight="1">
-      <c r="A19" s="14" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A20" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="22" t="s">
+      <c r="B20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" ht="36" customHeight="1">
-      <c r="A21" s="17" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="15" t="s">
+      <c r="B21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="63.75" customHeight="1">
-      <c r="A22" s="17" t="s">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1">
-      <c r="A23" s="17" t="s">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="B23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="B24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
@@ -1153,19 +1184,10 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="96" firstPageNumber="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>